<commit_message>
continue update KHDN and excel file, custom script
</commit_message>
<xml_diff>
--- a/data/userdata.xlsx
+++ b/data/userdata.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
-  <si>
-    <t>password</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
   <si>
     <t>userKHCN</t>
   </si>
@@ -39,42 +36,18 @@
     <t>fromaccountKHDN</t>
   </si>
   <si>
-    <t>abc123</t>
-  </si>
-  <si>
     <t>userKHDNnhap</t>
   </si>
   <si>
     <t>userKHDNduyet</t>
   </si>
   <si>
-    <t>authKHCN</t>
-  </si>
-  <si>
-    <t>authKHDN</t>
-  </si>
-  <si>
-    <t>SMS OTP</t>
-  </si>
-  <si>
-    <t>HDBank OTP</t>
-  </si>
-  <si>
     <t>autotestnhap</t>
   </si>
   <si>
     <t>autotestduyet</t>
   </si>
   <si>
-    <t>045704070000966 (CTY CP HOANG YEN) - VND</t>
-  </si>
-  <si>
-    <t>045704070000175 (DO THI LAN ANH) - VND</t>
-  </si>
-  <si>
-    <t>lananh2009</t>
-  </si>
-  <si>
     <t>minhson0907</t>
   </si>
   <si>
@@ -82,6 +55,27 @@
   </si>
   <si>
     <t>YXBwbGVpcGhvbmU2Uw==</t>
+  </si>
+  <si>
+    <t>045704070000966</t>
+  </si>
+  <si>
+    <t>YWJjMTIz</t>
+  </si>
+  <si>
+    <t>passKHDN_nhap</t>
+  </si>
+  <si>
+    <t>passKHDN_duyet</t>
+  </si>
+  <si>
+    <t>passKHCN</t>
+  </si>
+  <si>
+    <t>pincode</t>
+  </si>
+  <si>
+    <t>MTEyMjMz</t>
   </si>
 </sst>
 </file>
@@ -118,9 +112,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,48 +410,65 @@
     <col min="4" max="4" width="18.7109375" customWidth="1"/>
     <col min="5" max="5" width="60.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.28515625" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" customWidth="1"/>
+    <col min="7" max="8" width="25.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" t="s">
-        <v>0</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
         <v>16</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="G2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -470,7 +482,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -487,54 +499,54 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
       <c r="F1" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="G1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" t="s">
-        <v>9</v>
-      </c>
       <c r="H2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data for KHDN
</commit_message>
<xml_diff>
--- a/data/userdata.xlsx
+++ b/data/userdata.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonvm3\Desktop\cucumber-reporting-master\Checklistgolive_mB\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Auto\Checklistgolive_mB\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -13,7 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="son" sheetId="3" r:id="rId2"/>
+    <sheet name="userlive" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>userKHCN</t>
   </si>
@@ -42,12 +42,6 @@
     <t>userKHDNduyet</t>
   </si>
   <si>
-    <t>autotestnhap</t>
-  </si>
-  <si>
-    <t>autotestduyet</t>
-  </si>
-  <si>
     <t>minhson0907</t>
   </si>
   <si>
@@ -57,12 +51,6 @@
     <t>YXBwbGVpcGhvbmU2Uw==</t>
   </si>
   <si>
-    <t>045704070000966</t>
-  </si>
-  <si>
-    <t>YWJjMTIz</t>
-  </si>
-  <si>
     <t>passKHDN_nhap</t>
   </si>
   <si>
@@ -76,6 +64,21 @@
   </si>
   <si>
     <t>MTEyMjMz</t>
+  </si>
+  <si>
+    <t>hh_mk_doncap</t>
+  </si>
+  <si>
+    <t>hh_ck_doncap</t>
+  </si>
+  <si>
+    <t>016704070003846</t>
+  </si>
+  <si>
+    <t>QWJjMTIz</t>
+  </si>
+  <si>
+    <t>UXdlMTIz</t>
   </si>
 </sst>
 </file>
@@ -399,7 +402,7 @@
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,45 +433,45 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="I1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -482,7 +485,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -492,8 +495,8 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="60.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -514,39 +517,39 @@
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="G1" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H1" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update order bouquet and bonds
</commit_message>
<xml_diff>
--- a/data/userdata.xlsx
+++ b/data/userdata.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
   <si>
     <t>userKHCN</t>
   </si>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>UXdlMTIz</t>
+  </si>
+  <si>
+    <t>minhson0907</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>aGlnaGxhbmQxMFg=</t>
+  </si>
+  <si>
+    <t>002704070016025</t>
   </si>
 </sst>
 </file>
@@ -392,8 +404,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,7 +449,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>
@@ -446,6 +463,9 @@
       </c>
       <c r="E2" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>17</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
@@ -467,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -510,7 +530,9 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="C2" t="s">
         <v>10</v>
       </c>

</xml_diff>